<commit_message>
CRUD para alimentação do programa implementado
</commit_message>
<xml_diff>
--- a/cadastro_salao/data/agendamentos.xlsx
+++ b/cadastro_salao/data/agendamentos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>nome</t>
   </si>
@@ -49,67 +49,40 @@
     <t>tag</t>
   </si>
   <si>
-    <t>ruth</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
     <t>abraao</t>
   </si>
   <si>
     <t>abraaocursos2019@gmail.com</t>
   </si>
   <si>
-    <t>cobranca1@floraltextil.com.br</t>
-  </si>
-  <si>
-    <t>abraaocursos2017@gmail.com</t>
-  </si>
-  <si>
-    <t>85986862632</t>
-  </si>
-  <si>
-    <t>85986820652</t>
-  </si>
-  <si>
-    <t>Printura</t>
-  </si>
-  <si>
-    <t>Pacote Completo</t>
-  </si>
-  <si>
-    <t>Printura de cabelo com tinta temporária.</t>
-  </si>
-  <si>
-    <t>Cabelo + Barba + Printura com desconto especial.</t>
-  </si>
-  <si>
-    <t>Abraao</t>
-  </si>
-  <si>
-    <t>26/01/2026</t>
-  </si>
-  <si>
-    <t>26/12/2025</t>
-  </si>
-  <si>
-    <t>20/01/2026</t>
+    <t>Pintura</t>
+  </si>
+  <si>
+    <t>Pintura de cabelo com tinta temporária</t>
+  </si>
+  <si>
+    <t>Paulo</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>26/05/2026</t>
+  </si>
+  <si>
+    <t>25/01/2026</t>
   </si>
   <si>
     <t>20:00</t>
   </si>
   <si>
-    <t>20:20</t>
-  </si>
-  <si>
-    <t>2026-01-26T20:00:00</t>
-  </si>
-  <si>
-    <t>2025-12-26T20:00:00</t>
-  </si>
-  <si>
-    <t>2026-01-20T20:20:00</t>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>2026-05-26T20:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-25T15:00:00</t>
   </si>
   <si>
     <t>agendamento</t>
@@ -470,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,98 +489,69 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>85986820652</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
       <c r="F2">
         <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
+      <c r="C3">
+        <v>85986820652</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>15</v>
       </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>60</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotagem dos gráficos em um HTML implementado
</commit_message>
<xml_diff>
--- a/cadastro_salao/data/agendamentos.xlsx
+++ b/cadastro_salao/data/agendamentos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>nome</t>
   </si>
@@ -49,40 +49,151 @@
     <t>tag</t>
   </si>
   <si>
-    <t>abraao</t>
-  </si>
-  <si>
-    <t>abraaocursos2019@gmail.com</t>
-  </si>
-  <si>
-    <t>Pintura</t>
-  </si>
-  <si>
-    <t>Pintura de cabelo com tinta temporária</t>
+    <t>amanda conceição</t>
+  </si>
+  <si>
+    <t>ricardo gomes</t>
+  </si>
+  <si>
+    <t>evelin gomez</t>
+  </si>
+  <si>
+    <t>mateus borges</t>
+  </si>
+  <si>
+    <t>alexandre melo</t>
+  </si>
+  <si>
+    <t>rebeca azevedo</t>
+  </si>
+  <si>
+    <t>julia martins</t>
+  </si>
+  <si>
+    <t>natalia dias</t>
+  </si>
+  <si>
+    <t>amanda@hotmail.com</t>
+  </si>
+  <si>
+    <t>ricardogomes@hotmail.com</t>
+  </si>
+  <si>
+    <t>evelingomez@hotmail.com</t>
+  </si>
+  <si>
+    <t>mateusborges2011@gmail.com</t>
+  </si>
+  <si>
+    <t>alexandremelo2025@gmail.com</t>
+  </si>
+  <si>
+    <t>rebecaazevedo@gmail.com</t>
+  </si>
+  <si>
+    <t>juliamartins@bol.com</t>
+  </si>
+  <si>
+    <t>natalia@hotmail.com</t>
+  </si>
+  <si>
+    <t>85 90909-0909</t>
+  </si>
+  <si>
+    <t>85 99889-8181</t>
+  </si>
+  <si>
+    <t>85 99112-6532</t>
+  </si>
+  <si>
+    <t>85 91111-1111</t>
+  </si>
+  <si>
+    <t>85 98784-2525</t>
+  </si>
+  <si>
+    <t>85 99959-9999</t>
+  </si>
+  <si>
+    <t>85 94545-1364</t>
+  </si>
+  <si>
+    <t>85 91523-2021</t>
+  </si>
+  <si>
+    <t>Corte clássico</t>
+  </si>
+  <si>
+    <t>Dia do noivo</t>
+  </si>
+  <si>
+    <t>Barba e bigode</t>
+  </si>
+  <si>
+    <t>Tratamento capilar</t>
+  </si>
+  <si>
+    <t>Aparagem e modelagem tradicionais</t>
+  </si>
+  <si>
+    <t>Pacote completo com corte, barba, tratamento facial e relaxamento</t>
+  </si>
+  <si>
+    <t>Desenho e contorno da barba com toalha quente e finalização com balm</t>
+  </si>
+  <si>
+    <t>Lavagem especial com massagem e hidratação profunda para revitalização dos fios</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Abraão</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
   </si>
   <si>
     <t>Paulo</t>
   </si>
   <si>
-    <t>João</t>
-  </si>
-  <si>
-    <t>26/05/2026</t>
-  </si>
-  <si>
-    <t>25/01/2026</t>
-  </si>
-  <si>
-    <t>20:00</t>
+    <t>12/12/2025</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>09:45</t>
+  </si>
+  <si>
+    <t>10:45</t>
+  </si>
+  <si>
+    <t>11:00</t>
   </si>
   <si>
     <t>15:00</t>
   </si>
   <si>
-    <t>2026-05-26T20:00:00</t>
-  </si>
-  <si>
-    <t>2026-01-25T15:00:00</t>
+    <t>2025-12-12T09:00:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T10:00:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T09:45:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T10:45:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T11:00:00</t>
+  </si>
+  <si>
+    <t>2025-12-12T15:00:00</t>
   </si>
   <si>
     <t>agendamento</t>
@@ -443,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,69 +600,279 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>85986820652</v>
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>85986820652</v>
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+      <c r="G7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>